<commit_message>
add user, register user on fancy box. send mail to registered user.
</commit_message>
<xml_diff>
--- a/db_design.xlsx
+++ b/db_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="20120" windowHeight="7480" tabRatio="944" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="944" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cake_sessions" sheetId="4" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="117">
   <si>
     <t>NO</t>
     <phoneticPr fontId="2"/>
@@ -577,6 +577,15 @@
     <t>606: бэлэг бусад</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>TINYINT UNSIGNED</t>
+  </si>
+  <si>
+    <t>0: user, 1: admin</t>
+  </si>
 </sst>
 </file>
 
@@ -585,7 +594,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -628,6 +637,22 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="5">
@@ -834,7 +859,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -843,8 +868,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -979,6 +1006,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -995,6 +1034,26 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1037,38 +1096,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1096,11 +1123,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Calc Currency (0)" xfId="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Header1" xfId="2"/>
     <cellStyle name="Header2" xfId="3"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1827,40 +1859,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -1879,12 +1911,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -1901,10 +1933,10 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -1921,10 +1953,10 @@
       <c r="F7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="54"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="14">
       <c r="A8" s="4"/>
@@ -1953,33 +1985,33 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -1989,17 +2021,27 @@
         <v>1</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="A10:A11"/>
@@ -2007,16 +2049,6 @@
     <mergeCell ref="C10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:G11"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -2035,10 +2067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -2070,40 +2102,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -2122,12 +2154,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -2146,10 +2178,10 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -2168,39 +2200,41 @@
       <c r="F7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="54"/>
-    </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" ht="14">
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
+    </row>
+    <row r="8" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="10">
         <v>4</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>19</v>
+        <v>114</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>115</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="54"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="31">
+        <v>0</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A9" s="10">
         <v>5</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>19</v>
@@ -2208,19 +2242,21 @@
       <c r="D9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="F9" s="19"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="54"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A10" s="10">
         <v>6</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>19</v>
@@ -2230,37 +2266,37 @@
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="54"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
     </row>
     <row r="11" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A11" s="10">
         <v>7</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="52"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="54"/>
+      <c r="D11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="62"/>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A12" s="10">
         <v>8</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>19</v>
@@ -2270,17 +2306,17 @@
       <c r="F12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="54"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="62"/>
     </row>
     <row r="13" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A13" s="10">
         <v>9</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>19</v>
@@ -2290,17 +2326,17 @@
       <c r="F13" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="52"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A14" s="10">
         <v>10</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>19</v>
@@ -2310,107 +2346,113 @@
       <c r="F14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="62"/>
     </row>
     <row r="15" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A15" s="10">
         <v>11</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="30"/>
       <c r="F15" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="62"/>
     </row>
     <row r="16" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A16" s="10">
         <v>12</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="30"/>
       <c r="F16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="54"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="62"/>
     </row>
     <row r="17" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A17" s="10">
         <v>13</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="30"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="54"/>
+      <c r="F17" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="62"/>
     </row>
     <row r="18" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A18" s="10">
         <v>14</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="E18" s="30"/>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="28"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="62"/>
+    </row>
+    <row r="19" spans="1:10" s="18" customFormat="1" ht="14">
+      <c r="A19" s="10">
+        <v>15</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="54"/>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="62"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A20" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -2421,90 +2463,106 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A21" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="14">
+      <c r="A21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A22" s="40"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="12" customHeight="1">
+      <c r="A22" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A23" s="8">
-        <v>1</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="14">
+      <c r="A24" s="8">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
+  <mergeCells count="29">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="G14:J14"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G8:J8"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G13:J13"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
       <formula1>区分</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2517,7 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+    <sheetView topLeftCell="B42" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -2550,40 +2608,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -2602,12 +2660,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -2624,12 +2682,12 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:10" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -2646,12 +2704,12 @@
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A8" s="10">
@@ -2668,10 +2726,10 @@
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A9" s="10">
@@ -2688,10 +2746,10 @@
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A10" s="10">
@@ -2708,10 +2766,10 @@
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="51"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A11" s="10">
@@ -2728,10 +2786,10 @@
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="51"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A12" s="10">
@@ -2748,10 +2806,10 @@
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="51"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="59"/>
     </row>
     <row r="13" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A13" s="10">
@@ -2768,10 +2826,10 @@
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="51"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="59"/>
     </row>
     <row r="14" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A14" s="10">
@@ -2788,10 +2846,10 @@
       <c r="F14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A15" s="10">
@@ -2808,10 +2866,10 @@
       <c r="F15" s="21">
         <v>0</v>
       </c>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A16" s="10">
@@ -2828,10 +2886,10 @@
       <c r="F16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A17" s="10">
@@ -2892,10 +2950,10 @@
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="28"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="1:10" s="18" customFormat="1" ht="14">
       <c r="A20" s="10">
@@ -2912,10 +2970,10 @@
       <c r="F20" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" ht="14">
       <c r="A21" s="4"/>
@@ -2944,33 +3002,33 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59" t="s">
+      <c r="D23" s="46"/>
+      <c r="E23" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="14">
-      <c r="A24" s="40"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -2980,11 +3038,11 @@
         <v>1</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -3402,17 +3460,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="G14:J14"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
@@ -3425,11 +3477,17 @@
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G13:J13"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -3484,40 +3542,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:12" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -3536,12 +3594,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -3560,12 +3618,12 @@
       <c r="F6" s="21">
         <v>2</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -3620,17 +3678,17 @@
       <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="47" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="33"/>
@@ -3640,11 +3698,11 @@
       <c r="J10" s="68"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="34"/>
       <c r="G11" s="66"/>
       <c r="H11" s="67"/>
@@ -3656,8 +3714,8 @@
         <v>1</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="5"/>
       <c r="F12" s="35"/>
       <c r="G12" s="66"/>
@@ -3703,12 +3761,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G7:J18"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:E11"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="G5:J5"/>
@@ -3718,6 +3770,12 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G7:J18"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -3771,40 +3829,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:12" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -3823,12 +3881,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -3845,12 +3903,12 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -3905,17 +3963,17 @@
       <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="47" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="33"/>
@@ -3925,11 +3983,11 @@
       <c r="J10" s="68"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="34"/>
       <c r="G11" s="66"/>
       <c r="H11" s="67"/>
@@ -3941,8 +3999,8 @@
         <v>1</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="5"/>
       <c r="F12" s="35"/>
       <c r="G12" s="66"/>
@@ -3988,12 +4046,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G7:J18"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:D11"/>
@@ -4003,6 +4055,12 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G7:J18"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -4056,40 +4114,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:12" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -4108,12 +4166,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -4130,12 +4188,12 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -4190,17 +4248,17 @@
       <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="47" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="33"/>
@@ -4210,11 +4268,11 @@
       <c r="J10" s="68"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="34"/>
       <c r="G11" s="66"/>
       <c r="H11" s="67"/>
@@ -4226,8 +4284,8 @@
         <v>1</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="5"/>
       <c r="F12" s="35"/>
       <c r="G12" s="66"/>
@@ -4273,21 +4331,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G7:J18"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -4341,40 +4399,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:12" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -4393,12 +4451,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -4415,12 +4473,12 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="10">
@@ -4475,17 +4533,17 @@
       <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="47" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="33"/>
@@ -4495,11 +4553,11 @@
       <c r="J10" s="68"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="34"/>
       <c r="G11" s="66"/>
       <c r="H11" s="67"/>
@@ -4511,8 +4569,8 @@
         <v>1</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="5"/>
       <c r="F12" s="35"/>
       <c r="G12" s="66"/>
@@ -4558,21 +4616,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G7:J18"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -4621,40 +4679,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="10">
@@ -4673,12 +4731,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="10">
@@ -4695,12 +4753,12 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="4"/>
@@ -4721,27 +4779,27 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59" t="s">
+      <c r="D9" s="46"/>
+      <c r="E9" s="47" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="60"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:10">
@@ -4749,13 +4807,18 @@
         <v>1</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="5"/>
       <c r="F11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="G5:J5"/>
@@ -4765,11 +4828,6 @@
     <mergeCell ref="C9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -4823,40 +4881,40 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:12" s="18" customFormat="1" ht="14">
       <c r="A5" s="10">
@@ -4875,12 +4933,12 @@
         <v>9</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:12" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="10">
@@ -4935,17 +4993,17 @@
       <c r="J8" s="68"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59" t="s">
+      <c r="D9" s="46"/>
+      <c r="E9" s="47" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="33"/>
@@ -4955,11 +5013,11 @@
       <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="14">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="60"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="34"/>
       <c r="G10" s="66"/>
       <c r="H10" s="67"/>
@@ -4971,8 +5029,8 @@
         <v>1</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="5"/>
       <c r="F11" s="35"/>
       <c r="G11" s="66"/>
@@ -5018,12 +5076,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G6:J17"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:J4"/>
@@ -5032,6 +5084,12 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G6:J17"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">

</xml_diff>